<commit_message>
add files for sugarcane and cornstover eval
</commit_message>
<xml_diff>
--- a/incentives/incentives_info.xlsx
+++ b/incentives/incentives_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/Biorefinery-Tax-Incentives/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD207F37-BF2A-B54D-AFC7-52E895D900DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E981BEC-2785-9A4F-8371-D804E8475803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="73">
   <si>
     <t>property</t>
   </si>
@@ -54,9 +54,6 @@
     <t>sales</t>
   </si>
   <si>
-    <t>not sure how to incorporate into calculations</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>building_mats</t>
   </si>
   <si>
-    <t>determine whether to pass integer or array</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -241,6 +235,15 @@
   </si>
   <si>
     <t>Type of tax</t>
+  </si>
+  <si>
+    <t>corn or cellulosic feedstock only</t>
+  </si>
+  <si>
+    <t>second generation feedstocks only</t>
+  </si>
+  <si>
+    <t>grain feedstock only</t>
   </si>
 </sst>
 </file>
@@ -647,7 +650,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C2:C25"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,28 +667,28 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -695,10 +698,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
@@ -707,10 +710,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -721,10 +724,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
@@ -733,10 +736,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -746,10 +749,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
@@ -758,10 +761,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -771,10 +774,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
@@ -783,10 +786,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -796,10 +799,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
@@ -808,10 +811,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L6" s="5"/>
     </row>
@@ -820,10 +823,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>4</v>
@@ -832,10 +835,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="L7" s="3"/>
     </row>
@@ -844,10 +847,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
@@ -856,10 +859,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="I8" s="2"/>
       <c r="K8" s="4"/>
@@ -871,10 +871,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
@@ -883,10 +883,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="I9" s="2"/>
       <c r="K9" s="4"/>
@@ -898,10 +895,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -910,10 +907,10 @@
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L10" s="3"/>
     </row>
@@ -922,10 +919,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>6</v>
@@ -934,10 +931,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="7"/>
@@ -949,10 +946,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
@@ -961,10 +958,10 @@
         <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="4"/>
@@ -974,10 +971,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -986,10 +983,10 @@
         <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L13" s="5"/>
     </row>
@@ -998,10 +995,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
@@ -1010,10 +1007,10 @@
         <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="3"/>
@@ -1023,10 +1020,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -1035,10 +1032,13 @@
         <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="5"/>
@@ -1049,10 +1049,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -1061,10 +1061,10 @@
         <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="3"/>
@@ -1075,10 +1075,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -1087,10 +1087,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L17" s="3"/>
     </row>
@@ -1099,10 +1099,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
@@ -1111,10 +1111,10 @@
         <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L18" s="3"/>
     </row>
@@ -1123,10 +1123,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
@@ -1135,10 +1135,10 @@
         <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="3"/>
@@ -1149,10 +1149,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>6</v>
@@ -1161,10 +1161,10 @@
         <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="3"/>
@@ -1175,10 +1175,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -1187,10 +1187,13 @@
         <v>3</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="4"/>
@@ -1200,10 +1203,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>7</v>
@@ -1212,10 +1215,10 @@
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="3"/>
@@ -1225,10 +1228,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
@@ -1237,10 +1240,10 @@
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="3"/>
@@ -1251,10 +1254,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>7</v>
@@ -1263,10 +1266,13 @@
         <v>3</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="M24" s="6"/>
       <c r="O24" s="8"/>
@@ -1278,10 +1284,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>5</v>
@@ -1291,7 +1297,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="H25" s="1" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>